<commit_message>
Corrected tree DBH errors and re-ran script
</commit_message>
<xml_diff>
--- a/datasets/tree_DBH_hollows/input/Plot 02.xlsx
+++ b/datasets/tree_DBH_hollows/input/Plot 02.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickjolly/Desktop/tfn tree_hollows/input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickjolly/Desktop/tfn/DataScienceProject/datasets/tree_DBH_hollows/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9417B21E-F76F-274D-9709-6708DF247B06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10C09F27-0B89-4D44-9A25-A5EABEB202E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11940" yWindow="780" windowWidth="16860" windowHeight="15940" xr2:uid="{83F2F213-4E0F-A945-9AFE-A16589661716}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="37">
   <si>
     <t>Tree Number</t>
   </si>
@@ -67,12 +67,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>C11</t>
-  </si>
-  <si>
-    <t>C14</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
@@ -149,6 +143,9 @@
   </si>
   <si>
     <t>Circumference originally recorded</t>
+  </si>
+  <si>
+    <t>Change to 239 (only year 6 number not reecorded at year 0)</t>
   </si>
 </sst>
 </file>
@@ -519,8 +516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD91C6DE-F9D7-3846-9E20-4799F8402C19}">
   <dimension ref="A1:M81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="82" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="82" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -563,7 +560,7 @@
         <v>9</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
@@ -578,7 +575,7 @@
         <v>36.605636911135932</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F2">
         <v>6</v>
@@ -593,7 +590,7 @@
         <v>0</v>
       </c>
       <c r="J2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="M2" s="2">
         <v>115</v>
@@ -611,7 +608,7 @@
         <v>35.969017138768351</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F3">
         <v>4</v>
@@ -626,7 +623,7 @@
         <v>0</v>
       </c>
       <c r="J3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="M3" s="2">
         <v>113</v>
@@ -644,7 +641,7 @@
         <v>42.016904976260371</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F4">
         <v>5</v>
@@ -659,7 +656,7 @@
         <v>0</v>
       </c>
       <c r="J4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="M4" s="2">
         <v>132</v>
@@ -677,7 +674,7 @@
         <v>42.971834634811742</v>
       </c>
       <c r="E5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F5">
         <v>5</v>
@@ -692,7 +689,7 @@
         <v>0</v>
       </c>
       <c r="J5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="M5" s="2">
         <v>135</v>
@@ -710,7 +707,7 @@
         <v>38.515496228238675</v>
       </c>
       <c r="E6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F6">
         <v>4</v>
@@ -725,7 +722,7 @@
         <v>0</v>
       </c>
       <c r="J6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="M6" s="2">
         <v>121</v>
@@ -743,7 +740,7 @@
         <v>40.425355545341418</v>
       </c>
       <c r="E7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F7">
         <v>5</v>
@@ -758,7 +755,7 @@
         <v>0</v>
       </c>
       <c r="J7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M7" s="2">
         <v>127</v>
@@ -776,7 +773,7 @@
         <v>39.470425886790046</v>
       </c>
       <c r="E8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F8">
         <v>4</v>
@@ -791,7 +788,7 @@
         <v>0</v>
       </c>
       <c r="J8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="M8" s="2">
         <v>124</v>
@@ -809,7 +806,7 @@
         <v>49.019722472303762</v>
       </c>
       <c r="E9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F9">
         <v>5</v>
@@ -824,7 +821,7 @@
         <v>0</v>
       </c>
       <c r="J9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="M9" s="2">
         <v>154</v>
@@ -842,7 +839,7 @@
         <v>42.653524748627952</v>
       </c>
       <c r="E10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F10">
         <v>5</v>
@@ -857,7 +854,7 @@
         <v>0</v>
       </c>
       <c r="J10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="M10" s="2">
         <v>134</v>
@@ -875,7 +872,7 @@
         <v>44.245074179546904</v>
       </c>
       <c r="E11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F11">
         <v>5</v>
@@ -890,15 +887,15 @@
         <v>0</v>
       </c>
       <c r="J11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="M11" s="2">
         <v>139</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>10</v>
+      <c r="A12">
+        <v>224</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -908,7 +905,7 @@
         <v>38.515496228238675</v>
       </c>
       <c r="E12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F12">
         <v>4</v>
@@ -923,10 +920,10 @@
         <v>0</v>
       </c>
       <c r="J12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="K12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="M12" s="2">
         <v>121</v>
@@ -944,7 +941,7 @@
         <v>40.425355545341418</v>
       </c>
       <c r="E13" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F13">
         <v>5</v>
@@ -959,7 +956,7 @@
         <v>0</v>
       </c>
       <c r="J13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="M13" s="2">
         <v>127</v>
@@ -977,7 +974,7 @@
         <v>40.107045659157627</v>
       </c>
       <c r="E14" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F14">
         <v>5</v>
@@ -992,15 +989,15 @@
         <v>0</v>
       </c>
       <c r="J14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="M14" s="2">
         <v>126</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>11</v>
+      <c r="A15">
+        <v>239</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -1010,7 +1007,7 @@
         <v>36.923946797319722</v>
       </c>
       <c r="E15" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F15">
         <v>4</v>
@@ -1025,7 +1022,7 @@
         <v>0</v>
       </c>
       <c r="J15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="K15" t="s">
         <v>36</v>
@@ -1046,7 +1043,7 @@
         <v>38.515496228238675</v>
       </c>
       <c r="E16" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F16">
         <v>4</v>
@@ -1061,7 +1058,7 @@
         <v>0</v>
       </c>
       <c r="J16" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="M16" s="2">
         <v>121</v>
@@ -1079,7 +1076,7 @@
         <v>37.242256683503513</v>
       </c>
       <c r="E17" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F17">
         <v>4</v>
@@ -1094,7 +1091,7 @@
         <v>0</v>
       </c>
       <c r="J17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="M17" s="2">
         <v>117</v>
@@ -1112,7 +1109,7 @@
         <v>42.016904976260371</v>
       </c>
       <c r="E18" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F18">
         <v>5</v>
@@ -1127,7 +1124,7 @@
         <v>0</v>
       </c>
       <c r="J18" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="M18" s="2">
         <v>132</v>
@@ -1145,7 +1142,7 @@
         <v>37.560566569687303</v>
       </c>
       <c r="E19" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F19">
         <v>4</v>
@@ -1160,7 +1157,7 @@
         <v>0</v>
       </c>
       <c r="J19" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="M19" s="2">
         <v>118</v>
@@ -1178,7 +1175,7 @@
         <v>36.923946797319722</v>
       </c>
       <c r="E20" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F20">
         <v>4</v>
@@ -1193,7 +1190,7 @@
         <v>0</v>
       </c>
       <c r="J20" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="M20" s="2">
         <v>116</v>
@@ -1211,7 +1208,7 @@
         <v>34.0591578216656</v>
       </c>
       <c r="E21" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F21">
         <v>4</v>
@@ -1226,7 +1223,7 @@
         <v>0</v>
       </c>
       <c r="J21" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="M21" s="2">
         <v>107</v>
@@ -1243,13 +1240,13 @@
         <v>25.3</v>
       </c>
       <c r="E22" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F22">
         <v>2</v>
       </c>
       <c r="J22" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
@@ -1263,13 +1260,13 @@
         <v>22.5</v>
       </c>
       <c r="E23" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F23">
         <v>2</v>
       </c>
       <c r="J23" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
@@ -1283,13 +1280,13 @@
         <v>23.5</v>
       </c>
       <c r="E24" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F24">
         <v>2</v>
       </c>
       <c r="J24" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
@@ -1303,13 +1300,13 @@
         <v>21.5</v>
       </c>
       <c r="E25" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F25">
         <v>2</v>
       </c>
       <c r="J25" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
@@ -1323,13 +1320,13 @@
         <v>24</v>
       </c>
       <c r="E26" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F26">
         <v>2</v>
       </c>
       <c r="J26" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
@@ -1343,13 +1340,13 @@
         <v>28.1</v>
       </c>
       <c r="E27" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F27">
         <v>2</v>
       </c>
       <c r="J27" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
@@ -1363,13 +1360,13 @@
         <v>24.3</v>
       </c>
       <c r="E28" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F28">
         <v>2</v>
       </c>
       <c r="J28" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
@@ -1383,13 +1380,13 @@
         <v>29.5</v>
       </c>
       <c r="E29" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F29">
         <v>2</v>
       </c>
       <c r="J29" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
@@ -1403,13 +1400,13 @@
         <v>27</v>
       </c>
       <c r="E30" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F30">
         <v>2</v>
       </c>
       <c r="J30" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
@@ -1423,13 +1420,13 @@
         <v>25.5</v>
       </c>
       <c r="E31" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F31">
         <v>2</v>
       </c>
       <c r="J31" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
@@ -1443,7 +1440,7 @@
         <v>34.299999999999997</v>
       </c>
       <c r="E32" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F32">
         <v>3</v>
@@ -1469,7 +1466,7 @@
         <v>33.6</v>
       </c>
       <c r="E33" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F33">
         <v>3</v>
@@ -1492,10 +1489,10 @@
         <v>0</v>
       </c>
       <c r="D34">
-        <v>32.299999999999997</v>
+        <v>32.200000000000003</v>
       </c>
       <c r="E34" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F34">
         <v>3</v>
@@ -1521,7 +1518,7 @@
         <v>32.1</v>
       </c>
       <c r="E35" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F35">
         <v>3</v>
@@ -1547,7 +1544,7 @@
         <v>31.8</v>
       </c>
       <c r="E36" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F36">
         <v>3</v>
@@ -1573,7 +1570,7 @@
         <v>30.7</v>
       </c>
       <c r="E37" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F37">
         <v>3</v>
@@ -1599,7 +1596,7 @@
         <v>33.299999999999997</v>
       </c>
       <c r="E38" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F38">
         <v>3</v>
@@ -1625,7 +1622,7 @@
         <v>31</v>
       </c>
       <c r="E39" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F39">
         <v>3</v>
@@ -1651,7 +1648,7 @@
         <v>30.9</v>
       </c>
       <c r="E40" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F40">
         <v>3</v>
@@ -1677,7 +1674,7 @@
         <v>33.200000000000003</v>
       </c>
       <c r="E41" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F41">
         <v>3</v>
@@ -1700,13 +1697,13 @@
         <v>6</v>
       </c>
       <c r="C42" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D42">
         <v>38.9</v>
       </c>
       <c r="E42" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F42">
         <v>4</v>
@@ -1723,13 +1720,13 @@
         <v>6</v>
       </c>
       <c r="C43" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D43">
         <v>42.4</v>
       </c>
       <c r="E43" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F43">
         <v>5</v>
@@ -1746,13 +1743,13 @@
         <v>6</v>
       </c>
       <c r="C44" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D44">
         <v>39.9</v>
       </c>
       <c r="E44" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F44">
         <v>4</v>
@@ -1769,13 +1766,13 @@
         <v>6</v>
       </c>
       <c r="C45" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D45">
         <v>40.200000000000003</v>
       </c>
       <c r="E45" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F45">
         <v>5</v>
@@ -1792,13 +1789,13 @@
         <v>6</v>
       </c>
       <c r="C46" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D46">
         <v>52</v>
       </c>
       <c r="E46" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F46">
         <v>6</v>
@@ -1815,13 +1812,13 @@
         <v>6</v>
       </c>
       <c r="C47" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D47">
         <v>36.6</v>
       </c>
       <c r="E47" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F47">
         <v>4</v>
@@ -1838,13 +1835,13 @@
         <v>6</v>
       </c>
       <c r="C48" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D48">
         <v>41.6</v>
       </c>
       <c r="E48" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F48">
         <v>5</v>
@@ -1861,13 +1858,13 @@
         <v>6</v>
       </c>
       <c r="C49" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D49">
         <v>43.7</v>
       </c>
       <c r="E49" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F49">
         <v>5</v>
@@ -1884,13 +1881,13 @@
         <v>6</v>
       </c>
       <c r="C50" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D50">
         <v>43.3</v>
       </c>
       <c r="E50" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F50">
         <v>5</v>
@@ -1907,13 +1904,13 @@
         <v>6</v>
       </c>
       <c r="C51" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D51">
         <v>34.1</v>
       </c>
       <c r="E51" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F51">
         <v>4</v>
@@ -1930,13 +1927,13 @@
         <v>6</v>
       </c>
       <c r="C52" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D52">
         <v>39.9</v>
       </c>
       <c r="E52" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F52">
         <v>4</v>
@@ -1953,13 +1950,13 @@
         <v>6</v>
       </c>
       <c r="C53" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D53">
         <v>41.7</v>
       </c>
       <c r="E53" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F53">
         <v>5</v>
@@ -1976,13 +1973,13 @@
         <v>6</v>
       </c>
       <c r="C54" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D54">
         <v>37.799999999999997</v>
       </c>
       <c r="E54" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F54">
         <v>4</v>
@@ -1999,13 +1996,13 @@
         <v>6</v>
       </c>
       <c r="C55" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D55">
         <v>39.200000000000003</v>
       </c>
       <c r="E55" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F55">
         <v>4</v>
@@ -2022,13 +2019,13 @@
         <v>6</v>
       </c>
       <c r="C56" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D56">
         <v>51</v>
       </c>
       <c r="E56" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F56">
         <v>6</v>
@@ -2045,13 +2042,13 @@
         <v>6</v>
       </c>
       <c r="C57" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D57">
         <v>43.2</v>
       </c>
       <c r="E57" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F57">
         <v>5</v>
@@ -2068,13 +2065,13 @@
         <v>6</v>
       </c>
       <c r="C58" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D58">
         <v>46</v>
       </c>
       <c r="E58" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F58">
         <v>5</v>
@@ -2091,13 +2088,13 @@
         <v>6</v>
       </c>
       <c r="C59" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D59">
         <v>39.200000000000003</v>
       </c>
       <c r="E59" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F59">
         <v>4</v>
@@ -2114,13 +2111,13 @@
         <v>6</v>
       </c>
       <c r="C60" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D60">
         <v>36.4</v>
       </c>
       <c r="E60" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F60">
         <v>4</v>
@@ -2137,19 +2134,19 @@
         <v>6</v>
       </c>
       <c r="C61" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D61">
         <v>38.299999999999997</v>
       </c>
       <c r="E61" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F61">
         <v>4</v>
       </c>
       <c r="J61" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.2">
@@ -2160,13 +2157,13 @@
         <v>6</v>
       </c>
       <c r="C62" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D62">
         <v>26.6</v>
       </c>
       <c r="E62" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F62">
         <v>3</v>
@@ -2183,13 +2180,13 @@
         <v>6</v>
       </c>
       <c r="C63" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D63">
         <v>35.700000000000003</v>
       </c>
       <c r="E63" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F63">
         <v>4</v>
@@ -2206,13 +2203,13 @@
         <v>6</v>
       </c>
       <c r="C64" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D64">
         <v>23.7</v>
       </c>
       <c r="E64" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F64">
         <v>3</v>
@@ -2229,13 +2226,13 @@
         <v>6</v>
       </c>
       <c r="C65" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D65">
         <v>25</v>
       </c>
       <c r="E65" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F65">
         <v>3</v>
@@ -2252,13 +2249,13 @@
         <v>6</v>
       </c>
       <c r="C66" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D66">
         <v>35.299999999999997</v>
       </c>
       <c r="E66" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F66">
         <v>4</v>
@@ -2275,13 +2272,13 @@
         <v>6</v>
       </c>
       <c r="C67" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D67">
         <v>21.8</v>
       </c>
       <c r="E67" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F67">
         <v>3</v>
@@ -2298,13 +2295,13 @@
         <v>6</v>
       </c>
       <c r="C68" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D68">
         <v>33.700000000000003</v>
       </c>
       <c r="E68" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F68">
         <v>4</v>
@@ -2321,13 +2318,13 @@
         <v>6</v>
       </c>
       <c r="C69" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D69">
         <v>24.5</v>
       </c>
       <c r="E69" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F69">
         <v>3</v>
@@ -2344,13 +2341,13 @@
         <v>6</v>
       </c>
       <c r="C70" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D70">
         <v>32.6</v>
       </c>
       <c r="E70" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F70">
         <v>4</v>
@@ -2367,13 +2364,13 @@
         <v>6</v>
       </c>
       <c r="C71" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D71">
         <v>32.6</v>
       </c>
       <c r="E71" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F71">
         <v>4</v>
@@ -2390,13 +2387,13 @@
         <v>6</v>
       </c>
       <c r="C72" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D72">
         <v>28.6</v>
       </c>
       <c r="E72" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F72">
         <v>3</v>
@@ -2413,13 +2410,13 @@
         <v>6</v>
       </c>
       <c r="C73" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D73">
         <v>24.8</v>
       </c>
       <c r="E73" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F73">
         <v>3</v>
@@ -2436,13 +2433,13 @@
         <v>6</v>
       </c>
       <c r="C74" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D74">
         <v>30</v>
       </c>
       <c r="E74" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F74">
         <v>4</v>
@@ -2459,13 +2456,13 @@
         <v>6</v>
       </c>
       <c r="C75" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D75">
         <v>27.8</v>
       </c>
       <c r="E75" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F75">
         <v>3</v>
@@ -2482,13 +2479,13 @@
         <v>6</v>
       </c>
       <c r="C76" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D76">
         <v>32.299999999999997</v>
       </c>
       <c r="E76" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F76">
         <v>4</v>
@@ -2505,13 +2502,13 @@
         <v>6</v>
       </c>
       <c r="C77" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D77">
         <v>34.1</v>
       </c>
       <c r="E77" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F77">
         <v>4</v>
@@ -2528,13 +2525,13 @@
         <v>6</v>
       </c>
       <c r="C78" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D78">
         <v>26.2</v>
       </c>
       <c r="E78" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F78">
         <v>3</v>
@@ -2551,13 +2548,13 @@
         <v>6</v>
       </c>
       <c r="C79" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D79">
         <v>31.4</v>
       </c>
       <c r="E79" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F79">
         <v>4</v>
@@ -2574,13 +2571,13 @@
         <v>6</v>
       </c>
       <c r="C80" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D80">
         <v>31.2</v>
       </c>
       <c r="E80" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F80">
         <v>4</v>
@@ -2597,13 +2594,13 @@
         <v>6</v>
       </c>
       <c r="C81" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D81">
         <v>34.5</v>
       </c>
       <c r="E81" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F81">
         <v>4</v>

</xml_diff>